<commit_message>
feat[DE]: Add instance filtering based on metrics; refact[DE]: Renaming
</commit_message>
<xml_diff>
--- a/DataSetExplorerTests/DataFactories/TestData/BurningKnight1.xlsx
+++ b/DataSetExplorerTests/DataFactories/TestData/BurningKnight1.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ccadet\platform\DataSetExplorerTests\DataFactories\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC723AD8-2F20-466E-AC8F-D333E7C55274}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65FB782A-D2E1-44D7-8541-51209FA7C412}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Long Method" sheetId="1" r:id="rId1"/>
-    <sheet name="Large Class" sheetId="2" r:id="rId2"/>
+    <sheet name="Long_Method" sheetId="1" r:id="rId1"/>
+    <sheet name="Large_Class" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -1483,12 +1483,6 @@
     <t>Link</t>
   </si>
   <si>
-    <t>Large Class</t>
-  </si>
-  <si>
-    <t>Long Method</t>
-  </si>
-  <si>
     <t>Annotator ID</t>
   </si>
   <si>
@@ -1505,6 +1499,12 @@
   </si>
   <si>
     <t>Aseprite.AsepriteFile.AsepriteFile(string, ContentBuildLogger)</t>
+  </si>
+  <si>
+    <t>Large_Class</t>
+  </si>
+  <si>
+    <t>Long_Method</t>
   </si>
 </sst>
 </file>
@@ -2013,30 +2013,30 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G15" sqref="G15"/>
+      <selection pane="bottomLeft" activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4609375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="61.07421875" customWidth="1"/>
-    <col min="2" max="2" width="10.765625" style="19" customWidth="1"/>
-    <col min="3" max="3" width="10.765625" customWidth="1"/>
-    <col min="4" max="4" width="11.53515625" customWidth="1"/>
-    <col min="6" max="6" width="11.53515625" customWidth="1"/>
-    <col min="8" max="8" width="11.53515625" customWidth="1"/>
-    <col min="10" max="10" width="11.53515625" customWidth="1"/>
-    <col min="12" max="12" width="11.53515625" customWidth="1"/>
+    <col min="1" max="1" width="61.109375" customWidth="1"/>
+    <col min="2" max="2" width="10.77734375" style="19" customWidth="1"/>
+    <col min="3" max="3" width="10.77734375" customWidth="1"/>
+    <col min="4" max="4" width="11.5546875" customWidth="1"/>
+    <col min="6" max="6" width="11.5546875" customWidth="1"/>
+    <col min="8" max="8" width="11.5546875" customWidth="1"/>
+    <col min="10" max="10" width="11.5546875" customWidth="1"/>
+    <col min="12" max="12" width="11.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="15.45" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="D1" s="23" t="s">
         <v>0</v>
@@ -2051,12 +2051,12 @@
       <c r="L1" s="24"/>
       <c r="M1" s="24"/>
     </row>
-    <row r="2" spans="1:13" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A2" s="22" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="B2" s="22" t="s">
-        <v>484</v>
+        <v>490</v>
       </c>
       <c r="C2" s="22">
         <v>1</v>
@@ -2082,7 +2082,7 @@
       </c>
       <c r="M2" s="27"/>
     </row>
-    <row r="3" spans="1:13" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
@@ -2123,9 +2123,9 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
       <c r="B4" s="8"/>
       <c r="C4" s="5">
@@ -2156,9 +2156,9 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:13" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
       <c r="B5" s="8"/>
       <c r="C5" s="6">
@@ -2183,7 +2183,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:13" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:13" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>9</v>
       </c>
@@ -2213,7 +2213,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:13" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:13" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>11</v>
       </c>
@@ -2237,7 +2237,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:13" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:13" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>12</v>
       </c>
@@ -2261,7 +2261,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:13" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:13" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>13</v>
       </c>
@@ -2291,7 +2291,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:13" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:13" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>14</v>
       </c>
@@ -2321,7 +2321,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:13" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:13" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>15</v>
       </c>
@@ -2345,7 +2345,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:13" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:13" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
         <v>16</v>
       </c>
@@ -2369,7 +2369,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:13" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:13" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
         <v>17</v>
       </c>
@@ -2393,7 +2393,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:13" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:13" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
         <v>18</v>
       </c>
@@ -2417,7 +2417,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:13" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:13" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
         <v>19</v>
       </c>
@@ -2441,7 +2441,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="1:13" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:13" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
         <v>20</v>
       </c>
@@ -2465,7 +2465,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
         <v>21</v>
       </c>
@@ -2489,7 +2489,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="18" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
         <v>22</v>
       </c>
@@ -2513,7 +2513,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="19" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
         <v>23</v>
       </c>
@@ -2537,7 +2537,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="20" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
         <v>24</v>
       </c>
@@ -2561,7 +2561,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="21" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
         <v>25</v>
       </c>
@@ -2585,7 +2585,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="22" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
         <v>26</v>
       </c>
@@ -2609,7 +2609,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="23" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
         <v>27</v>
       </c>
@@ -2633,7 +2633,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="24" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="s">
         <v>28</v>
       </c>
@@ -2657,7 +2657,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="25" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A25" s="7" t="s">
         <v>29</v>
       </c>
@@ -2681,7 +2681,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="26" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A26" s="7" t="s">
         <v>30</v>
       </c>
@@ -2705,7 +2705,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="27" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A27" s="7" t="s">
         <v>31</v>
       </c>
@@ -2729,7 +2729,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="28" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A28" s="7" t="s">
         <v>32</v>
       </c>
@@ -2753,7 +2753,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="29" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A29" s="7" t="s">
         <v>33</v>
       </c>
@@ -2777,7 +2777,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="30" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A30" s="7" t="s">
         <v>378</v>
       </c>
@@ -2801,7 +2801,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="31" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A31" s="7" t="s">
         <v>34</v>
       </c>
@@ -2825,7 +2825,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="32" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A32" s="7" t="s">
         <v>35</v>
       </c>
@@ -2849,7 +2849,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="33" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A33" s="12" t="s">
         <v>36</v>
       </c>
@@ -2873,7 +2873,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="34" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A34" s="12" t="s">
         <v>37</v>
       </c>
@@ -2897,7 +2897,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="35" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A35" s="12" t="s">
         <v>38</v>
       </c>
@@ -2921,7 +2921,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="36" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A36" s="6" t="s">
         <v>39</v>
       </c>
@@ -2948,7 +2948,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="37" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A37" s="12" t="s">
         <v>40</v>
       </c>
@@ -2972,7 +2972,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="38" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A38" s="12" t="s">
         <v>379</v>
       </c>
@@ -2996,7 +2996,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="39" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A39" s="12" t="s">
         <v>41</v>
       </c>
@@ -3020,7 +3020,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="40" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A40" s="12" t="s">
         <v>42</v>
       </c>
@@ -3044,7 +3044,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="41" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A41" s="12" t="s">
         <v>43</v>
       </c>
@@ -3068,7 +3068,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="42" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A42" s="12" t="s">
         <v>44</v>
       </c>
@@ -3092,7 +3092,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="43" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A43" s="12" t="s">
         <v>45</v>
       </c>
@@ -3116,7 +3116,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="44" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A44" s="6" t="s">
         <v>46</v>
       </c>
@@ -3143,7 +3143,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="45" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A45" s="6" t="s">
         <v>47</v>
       </c>
@@ -3167,7 +3167,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="46" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A46" s="12" t="s">
         <v>48</v>
       </c>
@@ -3191,7 +3191,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="47" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A47" s="12" t="s">
         <v>49</v>
       </c>
@@ -3215,7 +3215,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="48" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A48" s="12" t="s">
         <v>50</v>
       </c>
@@ -3239,7 +3239,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="49" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A49" s="12" t="s">
         <v>51</v>
       </c>
@@ -3263,7 +3263,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="50" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A50" s="12" t="s">
         <v>52</v>
       </c>
@@ -3287,7 +3287,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="51" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A51" s="12" t="s">
         <v>53</v>
       </c>
@@ -3311,7 +3311,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="52" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A52" s="12" t="s">
         <v>54</v>
       </c>
@@ -3335,7 +3335,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="53" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A53" s="12" t="s">
         <v>55</v>
       </c>
@@ -3359,7 +3359,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="54" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A54" s="6" t="s">
         <v>56</v>
       </c>
@@ -3386,7 +3386,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="55" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A55" s="12" t="s">
         <v>57</v>
       </c>
@@ -3410,7 +3410,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="56" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A56" s="12" t="s">
         <v>380</v>
       </c>
@@ -3434,7 +3434,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="57" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A57" s="12" t="s">
         <v>58</v>
       </c>
@@ -3458,7 +3458,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="58" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A58" s="12" t="s">
         <v>381</v>
       </c>
@@ -3483,7 +3483,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="59" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A59" s="12" t="s">
         <v>382</v>
       </c>
@@ -3507,7 +3507,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="60" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A60" s="6" t="s">
         <v>59</v>
       </c>
@@ -3534,7 +3534,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="61" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A61" s="6" t="s">
         <v>60</v>
       </c>
@@ -3567,7 +3567,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="62" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A62" s="6" t="s">
         <v>61</v>
       </c>
@@ -3594,7 +3594,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="63" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A63" s="12" t="s">
         <v>62</v>
       </c>
@@ -3618,7 +3618,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="64" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A64" s="12" t="s">
         <v>63</v>
       </c>
@@ -3642,7 +3642,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="65" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A65" s="12" t="s">
         <v>64</v>
       </c>
@@ -3666,7 +3666,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="66" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A66" s="12" t="s">
         <v>65</v>
       </c>
@@ -3690,7 +3690,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="67" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A67" s="12" t="s">
         <v>66</v>
       </c>
@@ -3714,7 +3714,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="68" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A68" s="6" t="s">
         <v>67</v>
       </c>
@@ -3744,7 +3744,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="69" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A69" s="12" t="s">
         <v>68</v>
       </c>
@@ -3768,7 +3768,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="70" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A70" s="12" t="s">
         <v>69</v>
       </c>
@@ -3792,7 +3792,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="71" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A71" s="12" t="s">
         <v>70</v>
       </c>
@@ -3816,7 +3816,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="72" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A72" s="12" t="s">
         <v>71</v>
       </c>
@@ -3840,7 +3840,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="73" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A73" s="12" t="s">
         <v>72</v>
       </c>
@@ -3864,7 +3864,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="74" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A74" s="12" t="s">
         <v>73</v>
       </c>
@@ -3888,7 +3888,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="75" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A75" s="12" t="s">
         <v>74</v>
       </c>
@@ -3912,7 +3912,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="76" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A76" s="12" t="s">
         <v>75</v>
       </c>
@@ -3936,7 +3936,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="77" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A77" s="12" t="s">
         <v>76</v>
       </c>
@@ -3960,7 +3960,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="78" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A78" s="12" t="s">
         <v>77</v>
       </c>
@@ -3984,7 +3984,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="79" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A79" s="12" t="s">
         <v>78</v>
       </c>
@@ -4008,7 +4008,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="80" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A80" s="6" t="s">
         <v>79</v>
       </c>
@@ -4035,7 +4035,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="81" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A81" s="6" t="s">
         <v>80</v>
       </c>
@@ -4065,7 +4065,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="82" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A82" s="12" t="s">
         <v>81</v>
       </c>
@@ -4089,7 +4089,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="83" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A83" s="6" t="s">
         <v>82</v>
       </c>
@@ -4116,7 +4116,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="84" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A84" s="12" t="s">
         <v>83</v>
       </c>
@@ -4140,7 +4140,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="85" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A85" s="12" t="s">
         <v>84</v>
       </c>
@@ -4164,7 +4164,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="86" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A86" s="12" t="s">
         <v>85</v>
       </c>
@@ -4188,7 +4188,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="87" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A87" s="6" t="s">
         <v>86</v>
       </c>
@@ -4215,7 +4215,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="88" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A88" s="12" t="s">
         <v>383</v>
       </c>
@@ -4239,7 +4239,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="89" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A89" s="12" t="s">
         <v>87</v>
       </c>
@@ -4263,7 +4263,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="90" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A90" s="12" t="s">
         <v>88</v>
       </c>
@@ -4287,7 +4287,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="91" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A91" s="12" t="s">
         <v>89</v>
       </c>
@@ -4311,7 +4311,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="92" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A92" s="12" t="s">
         <v>90</v>
       </c>
@@ -4335,7 +4335,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="93" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A93" s="12" t="s">
         <v>384</v>
       </c>
@@ -4359,7 +4359,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="94" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A94" s="12" t="s">
         <v>91</v>
       </c>
@@ -4383,7 +4383,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="95" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A95" s="12" t="s">
         <v>385</v>
       </c>
@@ -4407,7 +4407,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="96" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A96" s="6" t="s">
         <v>92</v>
       </c>
@@ -4434,7 +4434,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="97" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A97" s="6" t="s">
         <v>93</v>
       </c>
@@ -4464,7 +4464,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="98" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A98" s="12" t="s">
         <v>386</v>
       </c>
@@ -4488,7 +4488,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="99" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A99" s="12" t="s">
         <v>94</v>
       </c>
@@ -4512,7 +4512,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="100" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A100" s="12" t="s">
         <v>95</v>
       </c>
@@ -4536,7 +4536,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="101" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A101" s="12" t="s">
         <v>96</v>
       </c>
@@ -4560,7 +4560,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="102" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A102" s="6" t="s">
         <v>97</v>
       </c>
@@ -4584,7 +4584,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="103" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A103" s="6" t="s">
         <v>98</v>
       </c>
@@ -4611,7 +4611,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="104" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A104" s="12" t="s">
         <v>99</v>
       </c>
@@ -4635,7 +4635,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="105" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A105" s="12" t="s">
         <v>100</v>
       </c>
@@ -4659,7 +4659,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="106" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A106" s="12" t="s">
         <v>387</v>
       </c>
@@ -4683,7 +4683,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="107" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A107" s="12" t="s">
         <v>101</v>
       </c>
@@ -4707,7 +4707,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="108" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A108" s="12" t="s">
         <v>102</v>
       </c>
@@ -4731,7 +4731,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="109" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A109" s="12" t="s">
         <v>388</v>
       </c>
@@ -4755,7 +4755,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="110" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A110" s="12" t="s">
         <v>103</v>
       </c>
@@ -4779,7 +4779,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="111" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A111" s="12" t="s">
         <v>104</v>
       </c>
@@ -4803,7 +4803,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="112" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A112" s="12" t="s">
         <v>389</v>
       </c>
@@ -4827,7 +4827,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="113" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A113" s="12" t="s">
         <v>105</v>
       </c>
@@ -4851,7 +4851,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="114" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A114" s="12" t="s">
         <v>390</v>
       </c>
@@ -4875,7 +4875,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="115" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A115" s="12" t="s">
         <v>106</v>
       </c>
@@ -4899,7 +4899,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="116" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A116" s="18" t="s">
         <v>391</v>
       </c>
@@ -4929,7 +4929,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="117" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A117" s="12" t="s">
         <v>107</v>
       </c>
@@ -4953,7 +4953,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="118" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A118" s="12" t="s">
         <v>108</v>
       </c>
@@ -4977,7 +4977,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="119" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A119" s="12" t="s">
         <v>392</v>
       </c>
@@ -5001,7 +5001,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="120" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A120" s="12" t="s">
         <v>109</v>
       </c>
@@ -5025,7 +5025,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="121" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A121" s="12" t="s">
         <v>110</v>
       </c>
@@ -5049,7 +5049,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="122" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A122" s="12" t="s">
         <v>393</v>
       </c>
@@ -5073,7 +5073,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="123" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A123" s="12" t="s">
         <v>111</v>
       </c>
@@ -5097,7 +5097,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="124" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A124" s="12" t="s">
         <v>394</v>
       </c>
@@ -5121,7 +5121,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="125" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A125" s="12" t="s">
         <v>112</v>
       </c>
@@ -5145,7 +5145,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="126" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A126" s="12" t="s">
         <v>113</v>
       </c>
@@ -5169,7 +5169,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="127" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A127" s="12" t="s">
         <v>395</v>
       </c>
@@ -5193,7 +5193,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="128" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A128" s="12" t="s">
         <v>114</v>
       </c>
@@ -5217,7 +5217,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="129" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A129" s="12" t="s">
         <v>115</v>
       </c>
@@ -5241,7 +5241,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="130" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A130" s="12" t="s">
         <v>396</v>
       </c>
@@ -5265,7 +5265,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="131" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A131" s="12" t="s">
         <v>116</v>
       </c>
@@ -5289,7 +5289,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="132" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A132" s="12" t="s">
         <v>117</v>
       </c>
@@ -5313,7 +5313,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="133" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A133" s="6" t="s">
         <v>118</v>
       </c>
@@ -5340,7 +5340,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="134" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A134" s="6" t="s">
         <v>119</v>
       </c>
@@ -5366,7 +5366,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="135" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A135" s="12" t="s">
         <v>397</v>
       </c>
@@ -5390,7 +5390,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="136" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A136" s="12" t="s">
         <v>120</v>
       </c>
@@ -5414,7 +5414,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="137" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A137" s="6" t="s">
         <v>121</v>
       </c>
@@ -5438,7 +5438,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="138" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A138" s="12" t="s">
         <v>398</v>
       </c>
@@ -5462,7 +5462,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="139" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A139" s="6" t="s">
         <v>122</v>
       </c>
@@ -5489,7 +5489,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="140" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A140" s="12" t="s">
         <v>399</v>
       </c>
@@ -5513,7 +5513,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="141" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A141" s="6" t="s">
         <v>123</v>
       </c>
@@ -5537,7 +5537,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="142" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A142" s="12" t="s">
         <v>400</v>
       </c>
@@ -5561,7 +5561,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="143" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A143" s="12" t="s">
         <v>124</v>
       </c>
@@ -5585,7 +5585,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="144" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A144" s="12" t="s">
         <v>401</v>
       </c>
@@ -5609,7 +5609,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="145" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A145" s="12" t="s">
         <v>125</v>
       </c>
@@ -5633,7 +5633,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="146" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A146" s="12" t="s">
         <v>126</v>
       </c>
@@ -5657,7 +5657,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="147" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A147" s="6" t="s">
         <v>127</v>
       </c>
@@ -5684,7 +5684,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="148" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A148" s="12" t="s">
         <v>128</v>
       </c>
@@ -5708,7 +5708,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="149" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A149" s="6" t="s">
         <v>129</v>
       </c>
@@ -5741,7 +5741,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="150" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A150" s="12" t="s">
         <v>130</v>
       </c>
@@ -5765,7 +5765,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="151" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A151" s="12" t="s">
         <v>131</v>
       </c>
@@ -5789,7 +5789,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="152" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A152" s="12" t="s">
         <v>132</v>
       </c>
@@ -5813,7 +5813,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="153" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A153" s="6" t="s">
         <v>133</v>
       </c>
@@ -5843,7 +5843,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="154" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A154" s="6" t="s">
         <v>134</v>
       </c>
@@ -5867,7 +5867,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="155" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A155" s="6" t="s">
         <v>135</v>
       </c>
@@ -5897,7 +5897,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="156" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A156" s="6" t="s">
         <v>136</v>
       </c>
@@ -5924,7 +5924,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="157" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A157" s="12" t="s">
         <v>137</v>
       </c>
@@ -5948,7 +5948,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="158" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A158" s="6" t="s">
         <v>138</v>
       </c>
@@ -5975,7 +5975,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="159" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A159" s="12" t="s">
         <v>402</v>
       </c>
@@ -5999,7 +5999,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="160" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A160" s="12" t="s">
         <v>403</v>
       </c>
@@ -6023,7 +6023,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="161" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A161" s="12" t="s">
         <v>139</v>
       </c>
@@ -6047,7 +6047,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="162" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A162" s="12" t="s">
         <v>404</v>
       </c>
@@ -6071,7 +6071,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="163" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A163" s="12" t="s">
         <v>140</v>
       </c>
@@ -6095,7 +6095,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="164" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A164" s="12" t="s">
         <v>141</v>
       </c>
@@ -6119,7 +6119,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="165" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A165" s="12" t="s">
         <v>142</v>
       </c>
@@ -6143,7 +6143,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="166" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A166" s="12" t="s">
         <v>143</v>
       </c>
@@ -6167,7 +6167,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="167" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A167" s="12" t="s">
         <v>144</v>
       </c>
@@ -6191,7 +6191,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="168" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A168" s="12" t="s">
         <v>145</v>
       </c>
@@ -6215,7 +6215,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="169" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A169" s="12" t="s">
         <v>146</v>
       </c>
@@ -6239,7 +6239,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="170" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A170" s="12" t="s">
         <v>147</v>
       </c>
@@ -6263,7 +6263,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="171" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A171" s="6" t="s">
         <v>148</v>
       </c>
@@ -6290,7 +6290,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="172" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A172" s="12" t="s">
         <v>149</v>
       </c>
@@ -6314,7 +6314,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="173" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A173" s="12" t="s">
         <v>150</v>
       </c>
@@ -6338,7 +6338,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="174" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A174" s="6" t="s">
         <v>151</v>
       </c>
@@ -6362,7 +6362,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="175" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A175" s="12" t="s">
         <v>152</v>
       </c>
@@ -6386,7 +6386,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="176" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A176" s="6" t="s">
         <v>153</v>
       </c>
@@ -6410,7 +6410,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="177" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A177" s="12" t="s">
         <v>154</v>
       </c>
@@ -6434,7 +6434,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="178" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A178" s="12" t="s">
         <v>405</v>
       </c>
@@ -6458,7 +6458,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="179" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A179" s="6" t="s">
         <v>155</v>
       </c>
@@ -6488,7 +6488,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="180" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A180" s="12" t="s">
         <v>156</v>
       </c>
@@ -6512,7 +6512,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="181" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A181" s="12" t="s">
         <v>157</v>
       </c>
@@ -6536,7 +6536,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="182" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A182" s="12" t="s">
         <v>158</v>
       </c>
@@ -6560,7 +6560,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="183" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A183" s="12" t="s">
         <v>159</v>
       </c>
@@ -6584,7 +6584,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="184" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A184" s="12" t="s">
         <v>160</v>
       </c>
@@ -6608,7 +6608,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="185" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A185" s="6" t="s">
         <v>161</v>
       </c>
@@ -6638,7 +6638,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="186" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A186" s="12" t="s">
         <v>406</v>
       </c>
@@ -6662,7 +6662,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="187" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A187" s="12" t="s">
         <v>162</v>
       </c>
@@ -6686,7 +6686,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="188" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A188" s="6" t="s">
         <v>163</v>
       </c>
@@ -6713,7 +6713,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="189" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A189" s="12" t="s">
         <v>164</v>
       </c>
@@ -6737,7 +6737,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="190" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A190" s="12" t="s">
         <v>165</v>
       </c>
@@ -6761,7 +6761,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="191" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="191" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A191" s="6" t="s">
         <v>166</v>
       </c>
@@ -6791,7 +6791,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="192" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A192" s="12" t="s">
         <v>167</v>
       </c>
@@ -6815,7 +6815,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="193" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A193" s="12" t="s">
         <v>168</v>
       </c>
@@ -6839,7 +6839,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="194" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="194" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A194" s="6" t="s">
         <v>169</v>
       </c>
@@ -6866,7 +6866,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="195" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="195" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A195" s="12" t="s">
         <v>170</v>
       </c>
@@ -6890,7 +6890,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="196" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="196" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A196" s="12" t="s">
         <v>171</v>
       </c>
@@ -6914,7 +6914,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="197" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="197" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A197" s="6" t="s">
         <v>172</v>
       </c>
@@ -6938,7 +6938,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="198" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="198" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A198" s="12" t="s">
         <v>173</v>
       </c>
@@ -6962,7 +6962,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="199" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="199" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A199" s="6" t="s">
         <v>174</v>
       </c>
@@ -6992,7 +6992,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="200" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="200" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A200" s="12" t="s">
         <v>175</v>
       </c>
@@ -7016,7 +7016,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="201" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="201" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A201" s="12" t="s">
         <v>176</v>
       </c>
@@ -7040,7 +7040,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="202" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="202" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A202" s="12" t="s">
         <v>177</v>
       </c>
@@ -7064,7 +7064,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="203" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="203" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A203" s="12" t="s">
         <v>178</v>
       </c>
@@ -7088,7 +7088,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="204" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="204" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A204" s="6" t="s">
         <v>179</v>
       </c>
@@ -7115,7 +7115,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="205" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="205" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A205" s="12" t="s">
         <v>180</v>
       </c>
@@ -7139,7 +7139,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="206" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="206" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A206" s="6" t="s">
         <v>181</v>
       </c>
@@ -7163,7 +7163,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="207" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="207" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A207" s="12" t="s">
         <v>182</v>
       </c>
@@ -7187,7 +7187,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="208" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="208" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A208" s="12" t="s">
         <v>183</v>
       </c>
@@ -7211,7 +7211,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="209" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="209" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A209" s="12" t="s">
         <v>184</v>
       </c>
@@ -7235,7 +7235,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="210" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="210" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A210" s="12" t="s">
         <v>185</v>
       </c>
@@ -7259,7 +7259,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="211" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="211" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A211" s="12" t="s">
         <v>186</v>
       </c>
@@ -7283,7 +7283,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="212" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="212" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A212" s="12" t="s">
         <v>187</v>
       </c>
@@ -7307,7 +7307,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="213" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="213" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A213" s="12" t="s">
         <v>188</v>
       </c>
@@ -7331,7 +7331,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="214" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="214" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A214" s="12" t="s">
         <v>189</v>
       </c>
@@ -7355,7 +7355,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="215" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="215" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A215" s="12" t="s">
         <v>190</v>
       </c>
@@ -7379,7 +7379,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="216" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="216" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A216" s="12" t="s">
         <v>191</v>
       </c>
@@ -7403,7 +7403,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="217" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="217" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A217" s="6" t="s">
         <v>192</v>
       </c>
@@ -7427,7 +7427,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="218" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="218" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A218" s="12" t="s">
         <v>193</v>
       </c>
@@ -7451,7 +7451,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="219" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="219" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A219" s="6" t="s">
         <v>194</v>
       </c>
@@ -7478,7 +7478,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="220" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="220" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A220" s="12" t="s">
         <v>195</v>
       </c>
@@ -7502,7 +7502,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="221" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="221" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A221" s="12" t="s">
         <v>196</v>
       </c>
@@ -7526,7 +7526,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="222" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="222" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A222" s="12" t="s">
         <v>197</v>
       </c>
@@ -7550,7 +7550,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="223" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="223" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A223" s="12" t="s">
         <v>198</v>
       </c>
@@ -7574,7 +7574,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="224" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="224" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A224" s="12" t="s">
         <v>199</v>
       </c>
@@ -7598,7 +7598,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="225" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="225" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A225" s="12" t="s">
         <v>200</v>
       </c>
@@ -7622,7 +7622,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="226" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="226" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A226" s="12" t="s">
         <v>201</v>
       </c>
@@ -7646,7 +7646,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="227" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="227" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A227" s="12" t="s">
         <v>202</v>
       </c>
@@ -7670,7 +7670,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="228" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="228" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A228" s="12" t="s">
         <v>203</v>
       </c>
@@ -7694,7 +7694,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="229" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="229" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A229" s="12" t="s">
         <v>204</v>
       </c>
@@ -7718,7 +7718,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="230" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="230" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A230" s="6" t="s">
         <v>205</v>
       </c>
@@ -7745,7 +7745,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="231" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="231" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A231" s="6" t="s">
         <v>206</v>
       </c>
@@ -7775,7 +7775,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="232" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="232" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A232" s="6" t="s">
         <v>207</v>
       </c>
@@ -7805,7 +7805,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="233" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="233" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A233" s="6" t="s">
         <v>208</v>
       </c>
@@ -7832,7 +7832,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="234" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="234" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A234" s="6" t="s">
         <v>209</v>
       </c>
@@ -7861,7 +7861,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="235" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="235" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A235" s="6" t="s">
         <v>210</v>
       </c>
@@ -7892,7 +7892,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="236" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="236" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A236" s="6" t="s">
         <v>211</v>
       </c>
@@ -7923,7 +7923,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="237" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="237" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A237" s="6" t="s">
         <v>212</v>
       </c>
@@ -7954,7 +7954,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="238" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="238" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A238" s="6" t="s">
         <v>213</v>
       </c>
@@ -7984,7 +7984,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="239" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="239" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A239" s="6" t="s">
         <v>214</v>
       </c>
@@ -8015,7 +8015,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="240" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="240" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A240" s="6" t="s">
         <v>215</v>
       </c>
@@ -8044,7 +8044,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="241" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="241" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A241" s="6" t="s">
         <v>216</v>
       </c>
@@ -8075,7 +8075,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="242" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="242" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A242" s="6" t="s">
         <v>217</v>
       </c>
@@ -8106,7 +8106,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="243" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="243" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A243" s="12" t="s">
         <v>218</v>
       </c>
@@ -8130,7 +8130,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="244" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="244" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A244" s="12" t="s">
         <v>219</v>
       </c>
@@ -8154,7 +8154,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="245" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="245" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A245" s="12" t="s">
         <v>220</v>
       </c>
@@ -8178,7 +8178,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="246" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="246" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A246" s="12" t="s">
         <v>221</v>
       </c>
@@ -8202,7 +8202,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="247" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="247" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A247" s="12" t="s">
         <v>222</v>
       </c>
@@ -8226,7 +8226,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="248" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="248" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A248" s="12" t="s">
         <v>223</v>
       </c>
@@ -8250,7 +8250,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="249" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="249" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A249" s="12" t="s">
         <v>224</v>
       </c>
@@ -8274,7 +8274,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="250" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="250" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A250" s="12" t="s">
         <v>225</v>
       </c>
@@ -8298,7 +8298,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="251" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="251" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A251" s="12" t="s">
         <v>226</v>
       </c>
@@ -8322,7 +8322,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="252" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="252" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A252" s="12" t="s">
         <v>227</v>
       </c>
@@ -8346,7 +8346,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="253" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="253" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A253" s="12" t="s">
         <v>228</v>
       </c>
@@ -8370,7 +8370,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="254" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="254" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A254" s="12" t="s">
         <v>229</v>
       </c>
@@ -8394,7 +8394,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="255" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="255" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A255" s="12" t="s">
         <v>230</v>
       </c>
@@ -8418,7 +8418,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="256" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="256" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A256" s="6" t="s">
         <v>231</v>
       </c>
@@ -8449,7 +8449,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="257" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="257" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A257" s="6" t="s">
         <v>232</v>
       </c>
@@ -8480,7 +8480,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="258" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="258" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A258" s="12" t="s">
         <v>233</v>
       </c>
@@ -8504,7 +8504,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="259" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="259" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A259" s="12" t="s">
         <v>234</v>
       </c>
@@ -8528,7 +8528,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="260" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="260" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A260" s="6" t="s">
         <v>235</v>
       </c>
@@ -8557,7 +8557,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="261" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="261" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A261" s="12" t="s">
         <v>236</v>
       </c>
@@ -8581,7 +8581,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="262" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="262" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A262" s="12" t="s">
         <v>237</v>
       </c>
@@ -8605,7 +8605,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="263" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="263" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A263" s="6" t="s">
         <v>238</v>
       </c>
@@ -8634,7 +8634,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="264" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="264" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A264" s="6" t="s">
         <v>239</v>
       </c>
@@ -8665,7 +8665,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="265" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="265" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A265" s="12" t="s">
         <v>240</v>
       </c>
@@ -8689,7 +8689,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="266" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="266" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A266" s="12" t="s">
         <v>241</v>
       </c>
@@ -8713,7 +8713,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="267" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="267" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A267" s="6" t="s">
         <v>242</v>
       </c>
@@ -8737,7 +8737,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="268" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="268" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A268" s="6" t="s">
         <v>243</v>
       </c>
@@ -8767,7 +8767,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="269" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="269" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A269" s="6" t="s">
         <v>244</v>
       </c>
@@ -8794,7 +8794,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="270" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="270" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A270" s="6" t="s">
         <v>407</v>
       </c>
@@ -8824,7 +8824,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="271" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="271" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A271" s="12" t="s">
         <v>245</v>
       </c>
@@ -8848,7 +8848,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="272" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="272" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A272" s="6" t="s">
         <v>246</v>
       </c>
@@ -8878,7 +8878,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="273" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="273" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A273" s="6" t="s">
         <v>247</v>
       </c>
@@ -8905,7 +8905,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="274" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="274" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A274" s="6" t="s">
         <v>248</v>
       </c>
@@ -8935,7 +8935,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="275" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="275" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A275" s="6" t="s">
         <v>249</v>
       </c>
@@ -8965,7 +8965,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="276" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="276" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A276" s="12" t="s">
         <v>250</v>
       </c>
@@ -8989,7 +8989,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="277" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="277" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A277" s="6" t="s">
         <v>251</v>
       </c>
@@ -9016,7 +9016,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="278" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="278" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A278" s="6" t="s">
         <v>252</v>
       </c>
@@ -9047,7 +9047,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="279" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="279" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A279" s="6" t="s">
         <v>253</v>
       </c>
@@ -9077,7 +9077,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="280" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="280" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A280" s="6" t="s">
         <v>254</v>
       </c>
@@ -9107,7 +9107,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="281" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="281" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A281" s="6" t="s">
         <v>255</v>
       </c>
@@ -9138,7 +9138,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="282" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="282" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A282" s="6" t="s">
         <v>256</v>
       </c>
@@ -9169,7 +9169,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="283" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="283" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A283" s="6" t="s">
         <v>257</v>
       </c>
@@ -9196,7 +9196,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="284" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="284" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A284" s="6" t="s">
         <v>258</v>
       </c>
@@ -9227,7 +9227,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="285" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="285" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A285" s="12" t="s">
         <v>259</v>
       </c>
@@ -9251,7 +9251,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="286" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="286" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A286" s="6" t="s">
         <v>260</v>
       </c>
@@ -9282,7 +9282,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="287" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="287" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A287" s="12" t="s">
         <v>261</v>
       </c>
@@ -9306,7 +9306,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="288" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="288" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A288" s="12" t="s">
         <v>262</v>
       </c>
@@ -9330,7 +9330,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="289" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="289" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A289" s="12" t="s">
         <v>263</v>
       </c>
@@ -9354,7 +9354,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="290" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="290" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A290" s="6" t="s">
         <v>264</v>
       </c>
@@ -9381,7 +9381,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="291" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="291" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A291" s="12" t="s">
         <v>265</v>
       </c>
@@ -9405,7 +9405,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="292" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="292" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A292" s="12" t="s">
         <v>266</v>
       </c>
@@ -9429,7 +9429,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="293" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="293" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A293" s="12" t="s">
         <v>267</v>
       </c>
@@ -9453,7 +9453,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="294" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="294" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A294" s="12" t="s">
         <v>268</v>
       </c>
@@ -9477,7 +9477,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="295" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="295" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A295" s="12" t="s">
         <v>269</v>
       </c>
@@ -9501,7 +9501,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="296" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="296" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A296" s="12" t="s">
         <v>270</v>
       </c>
@@ -9525,7 +9525,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="297" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="297" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A297" s="12" t="s">
         <v>271</v>
       </c>
@@ -9549,7 +9549,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="298" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="298" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A298" s="12" t="s">
         <v>272</v>
       </c>
@@ -9573,7 +9573,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="299" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="299" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A299" s="12" t="s">
         <v>273</v>
       </c>
@@ -9597,7 +9597,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="300" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="300" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A300" s="12" t="s">
         <v>274</v>
       </c>
@@ -9621,7 +9621,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="301" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="301" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A301" s="6" t="s">
         <v>275</v>
       </c>
@@ -9648,7 +9648,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="302" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="302" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A302" s="12" t="s">
         <v>276</v>
       </c>
@@ -9672,7 +9672,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="303" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="303" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A303" s="12" t="s">
         <v>277</v>
       </c>
@@ -9696,7 +9696,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="304" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="304" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A304" s="6" t="s">
         <v>278</v>
       </c>
@@ -9723,7 +9723,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="305" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="305" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A305" s="12" t="s">
         <v>279</v>
       </c>
@@ -9747,7 +9747,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="306" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="306" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A306" s="12" t="s">
         <v>280</v>
       </c>
@@ -9771,7 +9771,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="307" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="307" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A307" s="6" t="s">
         <v>281</v>
       </c>
@@ -9801,7 +9801,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="308" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="308" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A308" s="12" t="s">
         <v>282</v>
       </c>
@@ -9877,7 +9877,7 @@
       <formula1>"No,Yes"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2" xr:uid="{98654933-4757-475F-8AFA-1E1E6C61684F}">
-      <formula1>"Large Class, Long Method"</formula1>
+      <formula1>"Large_Class, Long_Method"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -9894,29 +9894,29 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="3" topLeftCell="A64" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H95" sqref="H95"/>
+      <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4609375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="37.3046875" customWidth="1"/>
-    <col min="2" max="2" width="10.765625" style="19" customWidth="1"/>
-    <col min="3" max="3" width="10.765625" customWidth="1"/>
-    <col min="4" max="4" width="11.53515625" customWidth="1"/>
-    <col min="6" max="6" width="11.53515625" customWidth="1"/>
-    <col min="8" max="8" width="11.53515625" customWidth="1"/>
-    <col min="10" max="10" width="11.53515625" customWidth="1"/>
+    <col min="1" max="1" width="37.33203125" customWidth="1"/>
+    <col min="2" max="2" width="10.77734375" style="19" customWidth="1"/>
+    <col min="3" max="3" width="10.77734375" customWidth="1"/>
+    <col min="4" max="4" width="11.5546875" customWidth="1"/>
+    <col min="6" max="6" width="11.5546875" customWidth="1"/>
+    <col min="8" max="8" width="11.5546875" customWidth="1"/>
+    <col min="10" max="10" width="11.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="D1" s="23" t="s">
         <v>0</v>
@@ -9929,12 +9929,12 @@
       <c r="J1" s="24"/>
       <c r="K1" s="24"/>
     </row>
-    <row r="2" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="22" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="B2" s="22" t="s">
-        <v>483</v>
+        <v>489</v>
       </c>
       <c r="C2" s="22">
         <v>1</v>
@@ -9956,7 +9956,7 @@
       </c>
       <c r="K2" s="27"/>
     </row>
-    <row r="3" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
@@ -9991,7 +9991,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>286</v>
       </c>
@@ -10012,7 +10012,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="11" t="s">
         <v>287</v>
       </c>
@@ -10039,7 +10039,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>288</v>
       </c>
@@ -10060,7 +10060,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>289</v>
       </c>
@@ -10081,7 +10081,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>290</v>
       </c>
@@ -10102,7 +10102,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>291</v>
       </c>
@@ -10123,7 +10123,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="12" t="s">
         <v>292</v>
       </c>
@@ -10144,7 +10144,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="s">
         <v>293</v>
       </c>
@@ -10165,7 +10165,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="12" t="s">
         <v>294</v>
       </c>
@@ -10186,7 +10186,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>295</v>
       </c>
@@ -10210,7 +10210,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
         <v>296</v>
       </c>
@@ -10234,7 +10234,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="12" t="s">
         <v>297</v>
       </c>
@@ -10255,7 +10255,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="12" t="s">
         <v>298</v>
       </c>
@@ -10276,7 +10276,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="12" t="s">
         <v>299</v>
       </c>
@@ -10297,7 +10297,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="18" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="12" t="s">
         <v>300</v>
       </c>
@@ -10318,7 +10318,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="19" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
         <v>301</v>
       </c>
@@ -10342,7 +10342,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="20" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="12" t="s">
         <v>302</v>
       </c>
@@ -10363,7 +10363,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="21" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
         <v>303</v>
       </c>
@@ -10387,7 +10387,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="22" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="12" t="s">
         <v>304</v>
       </c>
@@ -10408,7 +10408,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="23" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
         <v>305</v>
       </c>
@@ -10432,7 +10432,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="24" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
         <v>306</v>
       </c>
@@ -10456,7 +10456,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="25" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="12" t="s">
         <v>307</v>
       </c>
@@ -10477,7 +10477,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="26" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
         <v>308</v>
       </c>
@@ -10501,7 +10501,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="27" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="12" t="s">
         <v>309</v>
       </c>
@@ -10522,7 +10522,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="28" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="12" t="s">
         <v>310</v>
       </c>
@@ -10543,7 +10543,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="29" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
         <v>311</v>
       </c>
@@ -10573,7 +10573,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="30" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="12" t="s">
         <v>312</v>
       </c>
@@ -10594,7 +10594,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="31" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="12" t="s">
         <v>313</v>
       </c>
@@ -10615,7 +10615,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="32" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="5" t="s">
         <v>314</v>
       </c>
@@ -10639,7 +10639,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="33" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="5" t="s">
         <v>315</v>
       </c>
@@ -10663,7 +10663,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="34" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="12" t="s">
         <v>316</v>
       </c>
@@ -10684,7 +10684,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="35" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="5" t="s">
         <v>317</v>
       </c>
@@ -10708,7 +10708,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="36" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="12" t="s">
         <v>318</v>
       </c>
@@ -10729,7 +10729,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="37" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="5" t="s">
         <v>319</v>
       </c>
@@ -10759,7 +10759,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="38" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="12" t="s">
         <v>320</v>
       </c>
@@ -10780,7 +10780,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="39" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="12" t="s">
         <v>321</v>
       </c>
@@ -10801,7 +10801,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="40" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="12" t="s">
         <v>322</v>
       </c>
@@ -10822,7 +10822,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="41" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="12" t="s">
         <v>323</v>
       </c>
@@ -10843,7 +10843,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="42" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="12" t="s">
         <v>324</v>
       </c>
@@ -10864,7 +10864,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="43" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="5" t="s">
         <v>325</v>
       </c>
@@ -10888,7 +10888,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="44" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="12" t="s">
         <v>326</v>
       </c>
@@ -10909,7 +10909,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="45" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="12" t="s">
         <v>327</v>
       </c>
@@ -10930,7 +10930,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="46" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="12" t="s">
         <v>328</v>
       </c>
@@ -10951,7 +10951,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="47" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="12" t="s">
         <v>329</v>
       </c>
@@ -10972,7 +10972,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="48" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="12" t="s">
         <v>330</v>
       </c>
@@ -10993,7 +10993,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="49" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="5" t="s">
         <v>331</v>
       </c>
@@ -11017,7 +11017,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="50" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="12" t="s">
         <v>332</v>
       </c>
@@ -11038,7 +11038,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="51" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="12" t="s">
         <v>333</v>
       </c>
@@ -11059,7 +11059,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="52" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="12" t="s">
         <v>334</v>
       </c>
@@ -11080,7 +11080,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="53" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="12" t="s">
         <v>335</v>
       </c>
@@ -11101,7 +11101,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="54" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="12" t="s">
         <v>336</v>
       </c>
@@ -11122,7 +11122,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="55" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="12" t="s">
         <v>337</v>
       </c>
@@ -11143,7 +11143,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="56" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="5" t="s">
         <v>338</v>
       </c>
@@ -11167,7 +11167,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="57" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="12" t="s">
         <v>339</v>
       </c>
@@ -11188,7 +11188,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="58" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="5" t="s">
         <v>340</v>
       </c>
@@ -11212,7 +11212,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="59" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="12" t="s">
         <v>341</v>
       </c>
@@ -11233,7 +11233,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="60" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="12" t="s">
         <v>342</v>
       </c>
@@ -11254,7 +11254,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="61" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="12" t="s">
         <v>343</v>
       </c>
@@ -11275,7 +11275,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="62" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="12" t="s">
         <v>344</v>
       </c>
@@ -11296,7 +11296,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="63" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="12" t="s">
         <v>345</v>
       </c>
@@ -11317,7 +11317,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="64" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="5" t="s">
         <v>346</v>
       </c>
@@ -11341,7 +11341,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="65" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="5" t="s">
         <v>347</v>
       </c>
@@ -11368,7 +11368,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="66" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="12" t="s">
         <v>348</v>
       </c>
@@ -11389,7 +11389,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="67" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="12" t="s">
         <v>349</v>
       </c>
@@ -11410,7 +11410,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="68" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="12" t="s">
         <v>350</v>
       </c>
@@ -11431,7 +11431,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="69" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="12" t="s">
         <v>351</v>
       </c>
@@ -11452,7 +11452,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="70" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="12" t="s">
         <v>352</v>
       </c>
@@ -11473,7 +11473,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="71" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="12" t="s">
         <v>353</v>
       </c>
@@ -11494,7 +11494,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="72" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="5" t="s">
         <v>354</v>
       </c>
@@ -11515,7 +11515,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="73" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="12" t="s">
         <v>355</v>
       </c>
@@ -11536,7 +11536,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="74" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="12" t="s">
         <v>356</v>
       </c>
@@ -11557,7 +11557,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="75" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" s="12" t="s">
         <v>357</v>
       </c>
@@ -11578,7 +11578,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="76" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" s="12" t="s">
         <v>358</v>
       </c>
@@ -11599,7 +11599,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="77" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" s="12" t="s">
         <v>359</v>
       </c>
@@ -11620,7 +11620,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="78" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" s="12" t="s">
         <v>360</v>
       </c>
@@ -11641,7 +11641,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="79" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" s="5" t="s">
         <v>361</v>
       </c>
@@ -11662,7 +11662,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="80" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" s="5" t="s">
         <v>362</v>
       </c>
@@ -11683,7 +11683,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="81" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A81" s="5" t="s">
         <v>363</v>
       </c>
@@ -11707,7 +11707,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="82" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A82" s="5" t="s">
         <v>364</v>
       </c>
@@ -11771,7 +11771,7 @@
       <formula1>"No,Yes"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2" xr:uid="{D3AEB67F-07D5-4127-A35F-0419B9DAB47A}">
-      <formula1>"Large Class, Long Method"</formula1>
+      <formula1>"Large_Class, Long_Method"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>